<commit_message>
Correção remover avisos e nomes de variaveis
</commit_message>
<xml_diff>
--- a/Gerenciamento de Projeto/AGP - Planejamento e Controle do Projeto.xlsx
+++ b/Gerenciamento de Projeto/AGP - Planejamento e Controle do Projeto.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro\AGP\Gerenciamento de Projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D1A81E4-A036-423C-BA51-C04862F9D315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF6BF690-2B12-4CBA-A3EF-290D0E48B65E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="797" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="797" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Equipe" sheetId="10" r:id="rId1"/>
@@ -3398,9 +3398,6 @@
     <t>A priorização é importante para saber o que entregar primeiro ou desenvolver primeiro. O Owner ou o próprio cliente são importantes nessa decisão. Isso vai ajudar a planejar os Sprints.</t>
   </si>
   <si>
-    <t>Visão, modelo de caso de uso e plano</t>
-  </si>
-  <si>
     <t>sprints</t>
   </si>
   <si>
@@ -3569,18 +3566,6 @@
     <t>1.5 em média</t>
   </si>
   <si>
-    <t>Fase de Elaboração e inicio UC01</t>
-  </si>
-  <si>
-    <t>Finalizar UC01, UC02 e UC03</t>
-  </si>
-  <si>
-    <t>UC04, UC05, UC06</t>
-  </si>
-  <si>
-    <t>UC07, UC08</t>
-  </si>
-  <si>
     <t>Fase de Transição</t>
   </si>
   <si>
@@ -3606,6 +3591,21 @@
   </si>
   <si>
     <t>Dia 15</t>
+  </si>
+  <si>
+    <t>Fase de Elaboração</t>
+  </si>
+  <si>
+    <t>Fase de Construção 2 (UC04, UC05, UC06)</t>
+  </si>
+  <si>
+    <t>Fase de Construção 3 (UC07, UC08)</t>
+  </si>
+  <si>
+    <t>Fase de Construção 1 (Finalizar UC01, UC02 e UC03)</t>
+  </si>
+  <si>
+    <t>Fase de Iniciação</t>
   </si>
 </sst>
 </file>
@@ -4842,6 +4842,21 @@
     <xf numFmtId="0" fontId="28" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -4863,9 +4878,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -4877,18 +4889,6 @@
     </xf>
     <xf numFmtId="0" fontId="22" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -12862,7 +12862,7 @@
     </row>
     <row r="2" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A2" s="147" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B2" s="147"/>
       <c r="C2" s="147"/>
@@ -12883,21 +12883,21 @@
         <v>44</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C4" s="144" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C5" s="144" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -12905,10 +12905,10 @@
         <v>45</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C6" s="144" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -12916,10 +12916,10 @@
         <v>45</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C7" s="144" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -13044,19 +13044,19 @@
         <v>40</v>
       </c>
       <c r="M1" s="41" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="N1" s="41" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="O1" s="41" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="P1" s="41" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="Q1" s="41" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
@@ -13086,7 +13086,7 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="135" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B3" s="128">
         <v>1</v>
@@ -13111,7 +13111,7 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="136" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B4" s="128">
         <v>2</v>
@@ -13136,7 +13136,7 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="136" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B5" s="128">
         <v>3</v>
@@ -13163,7 +13163,7 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="136" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B6" s="128">
         <v>2</v>
@@ -13188,7 +13188,7 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="136" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B7" s="128">
         <v>1</v>
@@ -13213,7 +13213,7 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="135" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B8" s="128">
         <v>2</v>
@@ -13238,7 +13238,7 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="136" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B9" s="128">
         <v>2</v>
@@ -13265,7 +13265,7 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="136" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B10" s="128">
         <v>5</v>
@@ -13292,7 +13292,7 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="136" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B11" s="128">
         <v>3</v>
@@ -13319,7 +13319,7 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="136" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B12" s="128">
         <v>2</v>
@@ -13344,7 +13344,7 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="135" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B13" s="128">
         <v>1</v>
@@ -13369,7 +13369,7 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="136" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B14" s="128">
         <v>2</v>
@@ -13396,7 +13396,7 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="136" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B15" s="128">
         <v>3</v>
@@ -13423,7 +13423,7 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="136" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B16" s="128">
         <v>2</v>
@@ -13450,7 +13450,7 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="136" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B17" s="128">
         <v>1</v>
@@ -13855,7 +13855,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="135" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B3" s="128">
         <v>2</v>
@@ -13877,7 +13877,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="136" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B4" s="128">
         <v>2</v>
@@ -13897,7 +13897,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="136" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B5" s="128">
         <v>3</v>
@@ -13919,7 +13919,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="136" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B6" s="128">
         <v>2</v>
@@ -13939,7 +13939,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="136" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B7" s="128">
         <v>1</v>
@@ -13959,7 +13959,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="135" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B8" s="128">
         <v>1</v>
@@ -13979,7 +13979,7 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="136" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B9" s="128">
         <v>1</v>
@@ -13999,7 +13999,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="136" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B10" s="128">
         <v>2</v>
@@ -14019,7 +14019,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="136" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B11" s="128">
         <v>1</v>
@@ -14039,7 +14039,7 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="136" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B12" s="128">
         <v>1</v>
@@ -15989,7 +15989,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16016,7 +16016,7 @@
     </row>
     <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A4" s="27" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B4" s="141">
         <f>'Backlog Produto'!$D$76</f>
@@ -16078,7 +16078,7 @@
         <v>4.1000000000000005</v>
       </c>
       <c r="C9" s="27" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -16217,7 +16217,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L76"/>
   <sheetViews>
-    <sheetView topLeftCell="A57" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A50" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
@@ -16345,7 +16345,7 @@
         <v>1</v>
       </c>
       <c r="G5" s="117" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="H5" s="125">
         <v>5</v>
@@ -16381,7 +16381,7 @@
         <v>2</v>
       </c>
       <c r="G6" s="117" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="H6" s="125">
         <v>4</v>
@@ -16417,7 +16417,7 @@
         <v>3</v>
       </c>
       <c r="G7" s="117" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H7" s="125">
         <v>5</v>
@@ -16453,7 +16453,7 @@
         <v>4</v>
       </c>
       <c r="G8" s="117" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="H8" s="125">
         <v>4</v>
@@ -16489,7 +16489,7 @@
         <v>5</v>
       </c>
       <c r="G9" s="117" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H9" s="125">
         <v>7</v>
@@ -16525,7 +16525,7 @@
         <v>6</v>
       </c>
       <c r="G10" s="117" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="H10" s="125">
         <v>5</v>
@@ -16558,7 +16558,7 @@
         <v>7</v>
       </c>
       <c r="G11" s="117" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H11" s="125">
         <v>5</v>
@@ -16594,7 +16594,7 @@
         <v>8</v>
       </c>
       <c r="G12" s="117" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="H12" s="125">
         <v>4</v>
@@ -16669,7 +16669,7 @@
         <v>1</v>
       </c>
       <c r="C15" s="135" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D15" s="128">
         <v>2</v>
@@ -16693,7 +16693,7 @@
         <v>1</v>
       </c>
       <c r="C16" s="136" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D16" s="128">
         <v>2</v>
@@ -16898,7 +16898,7 @@
         <v>2</v>
       </c>
       <c r="C26" s="135" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D26" s="128">
         <v>1</v>
@@ -16968,7 +16968,7 @@
         <v>2</v>
       </c>
       <c r="C31" s="135" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D31" s="128">
         <v>1</v>
@@ -17050,7 +17050,7 @@
         <v>2</v>
       </c>
       <c r="C37" s="135" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D37" s="128">
         <v>1</v>
@@ -17064,7 +17064,7 @@
         <v>2</v>
       </c>
       <c r="C38" s="136" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D38" s="128">
         <v>2</v>
@@ -17078,7 +17078,7 @@
         <v>2</v>
       </c>
       <c r="C39" s="136" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D39" s="128">
         <v>3</v>
@@ -17092,7 +17092,7 @@
         <v>2</v>
       </c>
       <c r="C40" s="136" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D40" s="128">
         <v>2</v>
@@ -17106,7 +17106,7 @@
         <v>2</v>
       </c>
       <c r="C41" s="136" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D41" s="128">
         <v>1</v>
@@ -17120,7 +17120,7 @@
         <v>2</v>
       </c>
       <c r="C42" s="135" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D42" s="128">
         <v>2</v>
@@ -17134,7 +17134,7 @@
         <v>2</v>
       </c>
       <c r="C43" s="136" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D43" s="128">
         <v>2</v>
@@ -17148,7 +17148,7 @@
         <v>2</v>
       </c>
       <c r="C44" s="136" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D44" s="128">
         <v>5</v>
@@ -17162,7 +17162,7 @@
         <v>2</v>
       </c>
       <c r="C45" s="136" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D45" s="128">
         <v>3</v>
@@ -17176,7 +17176,7 @@
         <v>2</v>
       </c>
       <c r="C46" s="136" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D46" s="128">
         <v>2</v>
@@ -17190,7 +17190,7 @@
         <v>2</v>
       </c>
       <c r="C47" s="135" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D47" s="128">
         <v>1</v>
@@ -17204,7 +17204,7 @@
         <v>2</v>
       </c>
       <c r="C48" s="136" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D48" s="128">
         <v>2</v>
@@ -17218,7 +17218,7 @@
         <v>2</v>
       </c>
       <c r="C49" s="136" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D49" s="128">
         <v>3</v>
@@ -17232,7 +17232,7 @@
         <v>2</v>
       </c>
       <c r="C50" s="136" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D50" s="128">
         <v>2</v>
@@ -17246,7 +17246,7 @@
         <v>2</v>
       </c>
       <c r="C51" s="136" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D51" s="128">
         <v>1</v>
@@ -17272,7 +17272,7 @@
         <v>2</v>
       </c>
       <c r="C53" s="135" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D53" s="128">
         <v>2</v>
@@ -17286,7 +17286,7 @@
         <v>2</v>
       </c>
       <c r="C54" s="136" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D54" s="128">
         <v>2</v>
@@ -17300,7 +17300,7 @@
         <v>2</v>
       </c>
       <c r="C55" s="136" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D55" s="128">
         <v>3</v>
@@ -17314,7 +17314,7 @@
         <v>2</v>
       </c>
       <c r="C56" s="136" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D56" s="128">
         <v>2</v>
@@ -17328,7 +17328,7 @@
         <v>2</v>
       </c>
       <c r="C57" s="136" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D57" s="128">
         <v>1</v>
@@ -17342,7 +17342,7 @@
         <v>2</v>
       </c>
       <c r="C58" s="135" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D58" s="128">
         <v>1</v>
@@ -17356,7 +17356,7 @@
         <v>2</v>
       </c>
       <c r="C59" s="136" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D59" s="128">
         <v>1</v>
@@ -17370,7 +17370,7 @@
         <v>2</v>
       </c>
       <c r="C60" s="136" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D60" s="128">
         <v>2</v>
@@ -17384,7 +17384,7 @@
         <v>2</v>
       </c>
       <c r="C61" s="136" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D61" s="128">
         <v>1</v>
@@ -17398,7 +17398,7 @@
         <v>2</v>
       </c>
       <c r="C62" s="136" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D62" s="128">
         <v>1</v>
@@ -17608,8 +17608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" zoomScale="127" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
@@ -17671,7 +17671,7 @@
     <row r="3" spans="1:11" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A3" s="79"/>
       <c r="B3" s="80" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C3" s="168" t="s">
         <v>71</v>
@@ -17727,7 +17727,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="87" t="s">
-        <v>242</v>
+        <v>311</v>
       </c>
       <c r="C5" s="88">
         <v>45553</v>
@@ -17739,7 +17739,7 @@
         <v>12</v>
       </c>
       <c r="F5" s="90" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G5" s="88">
         <v>45553</v>
@@ -17758,7 +17758,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="87" t="s">
-        <v>299</v>
+        <v>307</v>
       </c>
       <c r="C6" s="88">
         <v>45560</v>
@@ -17770,7 +17770,7 @@
         <v>32</v>
       </c>
       <c r="F6" s="90" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G6" s="88">
         <v>45560</v>
@@ -17789,7 +17789,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="87" t="s">
-        <v>300</v>
+        <v>310</v>
       </c>
       <c r="C7" s="88">
         <v>45572</v>
@@ -17801,7 +17801,7 @@
         <v>25</v>
       </c>
       <c r="F7" s="90" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G7" s="88">
         <v>45572</v>
@@ -17820,7 +17820,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="87" t="s">
-        <v>301</v>
+        <v>308</v>
       </c>
       <c r="C8" s="88">
         <v>45579</v>
@@ -17832,7 +17832,7 @@
         <v>33</v>
       </c>
       <c r="F8" s="90" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G8" s="88">
         <v>45580</v>
@@ -17851,7 +17851,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="87" t="s">
-        <v>302</v>
+        <v>309</v>
       </c>
       <c r="C9" s="88">
         <v>45595</v>
@@ -17863,7 +17863,7 @@
         <v>22</v>
       </c>
       <c r="F9" s="90" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G9" s="88">
         <v>45596</v>
@@ -17882,7 +17882,7 @@
         <v>6</v>
       </c>
       <c r="B10" s="87" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="C10" s="88">
         <v>45609</v>
@@ -17894,7 +17894,7 @@
         <v>40</v>
       </c>
       <c r="F10" s="90" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G10" s="88">
         <v>45610</v>
@@ -19031,10 +19031,10 @@
       </c>
     </row>
     <row r="33" spans="1:11" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D33" s="172" t="s">
+      <c r="D33" s="177" t="s">
         <v>109</v>
       </c>
-      <c r="E33" s="173"/>
+      <c r="E33" s="178"/>
     </row>
     <row r="34" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="D34" s="62">
@@ -19086,137 +19086,137 @@
     </row>
     <row r="40" spans="1:11" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="41" spans="1:11" s="54" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="180" t="s">
+      <c r="A41" s="184" t="s">
         <v>116</v>
       </c>
-      <c r="B41" s="180"/>
-      <c r="C41" s="180"/>
-      <c r="D41" s="180"/>
-      <c r="E41" s="180"/>
-      <c r="F41" s="180"/>
-      <c r="G41" s="180"/>
-      <c r="H41" s="180"/>
-      <c r="I41" s="180"/>
-      <c r="J41" s="180"/>
-      <c r="K41" s="180"/>
+      <c r="B41" s="184"/>
+      <c r="C41" s="184"/>
+      <c r="D41" s="184"/>
+      <c r="E41" s="184"/>
+      <c r="F41" s="184"/>
+      <c r="G41" s="184"/>
+      <c r="H41" s="184"/>
+      <c r="I41" s="184"/>
+      <c r="J41" s="184"/>
+      <c r="K41" s="184"/>
     </row>
     <row r="42" spans="1:11" s="54" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="181" t="s">
+      <c r="A42" s="185" t="s">
         <v>117</v>
       </c>
-      <c r="B42" s="181"/>
-      <c r="C42" s="181"/>
-      <c r="D42" s="181"/>
-      <c r="E42" s="181"/>
-      <c r="F42" s="181"/>
-      <c r="G42" s="181"/>
-      <c r="H42" s="181"/>
-      <c r="I42" s="181"/>
-      <c r="J42" s="181"/>
-      <c r="K42" s="181"/>
+      <c r="B42" s="185"/>
+      <c r="C42" s="185"/>
+      <c r="D42" s="185"/>
+      <c r="E42" s="185"/>
+      <c r="F42" s="185"/>
+      <c r="G42" s="185"/>
+      <c r="H42" s="185"/>
+      <c r="I42" s="185"/>
+      <c r="J42" s="185"/>
+      <c r="K42" s="185"/>
     </row>
     <row r="43" spans="1:11" s="54" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="182" t="s">
+      <c r="A43" s="186" t="s">
         <v>131</v>
       </c>
-      <c r="B43" s="182"/>
-      <c r="C43" s="182"/>
-      <c r="D43" s="182"/>
-      <c r="E43" s="182"/>
-      <c r="F43" s="182"/>
-      <c r="G43" s="182"/>
-      <c r="H43" s="182"/>
-      <c r="I43" s="182"/>
-      <c r="J43" s="182"/>
-      <c r="K43" s="182"/>
+      <c r="B43" s="186"/>
+      <c r="C43" s="186"/>
+      <c r="D43" s="186"/>
+      <c r="E43" s="186"/>
+      <c r="F43" s="186"/>
+      <c r="G43" s="186"/>
+      <c r="H43" s="186"/>
+      <c r="I43" s="186"/>
+      <c r="J43" s="186"/>
+      <c r="K43" s="186"/>
     </row>
     <row r="44" spans="1:11" s="54" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="183" t="s">
+      <c r="A44" s="187" t="s">
         <v>118</v>
       </c>
-      <c r="B44" s="183"/>
-      <c r="C44" s="183"/>
-      <c r="D44" s="183"/>
-      <c r="E44" s="183"/>
-      <c r="F44" s="183"/>
-      <c r="G44" s="183"/>
-      <c r="H44" s="183"/>
-      <c r="I44" s="183"/>
-      <c r="J44" s="183"/>
-      <c r="K44" s="183"/>
+      <c r="B44" s="187"/>
+      <c r="C44" s="187"/>
+      <c r="D44" s="187"/>
+      <c r="E44" s="187"/>
+      <c r="F44" s="187"/>
+      <c r="G44" s="187"/>
+      <c r="H44" s="187"/>
+      <c r="I44" s="187"/>
+      <c r="J44" s="187"/>
+      <c r="K44" s="187"/>
     </row>
     <row r="45" spans="1:11" ht="9" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="46" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="174" t="s">
+      <c r="A46" s="179" t="s">
         <v>119</v>
       </c>
-      <c r="B46" s="175"/>
-      <c r="C46" s="175"/>
-      <c r="D46" s="175"/>
-      <c r="E46" s="175"/>
-      <c r="F46" s="175"/>
-      <c r="G46" s="175"/>
-      <c r="H46" s="175"/>
-      <c r="I46" s="175"/>
-      <c r="J46" s="175"/>
-      <c r="K46" s="175"/>
+      <c r="B46" s="180"/>
+      <c r="C46" s="180"/>
+      <c r="D46" s="180"/>
+      <c r="E46" s="180"/>
+      <c r="F46" s="180"/>
+      <c r="G46" s="180"/>
+      <c r="H46" s="180"/>
+      <c r="I46" s="180"/>
+      <c r="J46" s="180"/>
+      <c r="K46" s="180"/>
     </row>
     <row r="47" spans="1:11" s="66" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="76" t="s">
         <v>120</v>
       </c>
       <c r="B47" s="75"/>
-      <c r="C47" s="176" t="s">
+      <c r="C47" s="181" t="s">
         <v>121</v>
       </c>
-      <c r="D47" s="176"/>
-      <c r="E47" s="176"/>
-      <c r="F47" s="176"/>
-      <c r="G47" s="176"/>
-      <c r="H47" s="176"/>
-      <c r="I47" s="176"/>
-      <c r="J47" s="176"/>
-      <c r="K47" s="176"/>
+      <c r="D47" s="181"/>
+      <c r="E47" s="181"/>
+      <c r="F47" s="181"/>
+      <c r="G47" s="181"/>
+      <c r="H47" s="181"/>
+      <c r="I47" s="181"/>
+      <c r="J47" s="181"/>
+      <c r="K47" s="181"/>
     </row>
     <row r="48" spans="1:11" s="67" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="179"/>
-      <c r="B48" s="179" t="s">
+      <c r="A48" s="174"/>
+      <c r="B48" s="174" t="s">
         <v>130</v>
       </c>
-      <c r="C48" s="179" t="s">
+      <c r="C48" s="174" t="s">
         <v>122</v>
       </c>
-      <c r="D48" s="179" t="s">
+      <c r="D48" s="174" t="s">
         <v>123</v>
       </c>
-      <c r="E48" s="179" t="s">
+      <c r="E48" s="174" t="s">
         <v>94</v>
       </c>
-      <c r="F48" s="179" t="s">
+      <c r="F48" s="174" t="s">
         <v>124</v>
       </c>
-      <c r="G48" s="179" t="s">
+      <c r="G48" s="174" t="s">
         <v>98</v>
       </c>
-      <c r="H48" s="186" t="s">
+      <c r="H48" s="175" t="s">
         <v>125</v>
       </c>
-      <c r="I48" s="187"/>
-      <c r="J48" s="187"/>
-      <c r="K48" s="187"/>
+      <c r="I48" s="176"/>
+      <c r="J48" s="176"/>
+      <c r="K48" s="176"/>
     </row>
     <row r="49" spans="1:11" s="67" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="179"/>
-      <c r="B49" s="179"/>
-      <c r="C49" s="179"/>
-      <c r="D49" s="179"/>
-      <c r="E49" s="179"/>
-      <c r="F49" s="179"/>
-      <c r="G49" s="179"/>
-      <c r="H49" s="177" t="s">
+      <c r="A49" s="174"/>
+      <c r="B49" s="174"/>
+      <c r="C49" s="174"/>
+      <c r="D49" s="174"/>
+      <c r="E49" s="174"/>
+      <c r="F49" s="174"/>
+      <c r="G49" s="174"/>
+      <c r="H49" s="182" t="s">
         <v>126</v>
       </c>
-      <c r="I49" s="178"/>
+      <c r="I49" s="183"/>
       <c r="J49" s="68" t="s">
         <v>127</v>
       </c>
@@ -19247,8 +19247,8 @@
       <c r="G50" s="70" t="s">
         <v>99</v>
       </c>
-      <c r="H50" s="184"/>
-      <c r="I50" s="185"/>
+      <c r="H50" s="172"/>
+      <c r="I50" s="173"/>
       <c r="J50" s="74"/>
       <c r="K50" s="74" t="s">
         <v>133</v>
@@ -19259,7 +19259,7 @@
         <v>2</v>
       </c>
       <c r="B51" s="96" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C51" s="69">
         <v>45553</v>
@@ -19405,8 +19405,8 @@
         <v>#VALUE!</v>
       </c>
       <c r="G59" s="70"/>
-      <c r="H59" s="184"/>
-      <c r="I59" s="185"/>
+      <c r="H59" s="172"/>
+      <c r="I59" s="173"/>
       <c r="J59" s="74"/>
       <c r="K59" s="74"/>
     </row>
@@ -19421,22 +19421,13 @@
         <v>#VALUE!</v>
       </c>
       <c r="G60" s="70"/>
-      <c r="H60" s="184"/>
-      <c r="I60" s="185"/>
+      <c r="H60" s="172"/>
+      <c r="I60" s="173"/>
       <c r="J60" s="74"/>
       <c r="K60" s="74"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="H50:I50"/>
-    <mergeCell ref="H59:I59"/>
-    <mergeCell ref="H60:I60"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="E48:E49"/>
-    <mergeCell ref="F48:F49"/>
-    <mergeCell ref="G48:G49"/>
-    <mergeCell ref="H48:K48"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="D33:E33"/>
     <mergeCell ref="A46:K46"/>
@@ -19448,6 +19439,15 @@
     <mergeCell ref="A42:K42"/>
     <mergeCell ref="A43:K43"/>
     <mergeCell ref="A44:K44"/>
+    <mergeCell ref="H50:I50"/>
+    <mergeCell ref="H59:I59"/>
+    <mergeCell ref="H60:I60"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="E48:E49"/>
+    <mergeCell ref="F48:F49"/>
+    <mergeCell ref="G48:G49"/>
+    <mergeCell ref="H48:K48"/>
   </mergeCells>
   <conditionalFormatting sqref="F50:F60">
     <cfRule type="cellIs" dxfId="4" priority="1" stopIfTrue="1" operator="equal">
@@ -19499,7 +19499,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="188" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B1" s="189"/>
       <c r="C1" s="189"/>
@@ -19518,13 +19518,13 @@
         <v>220</v>
       </c>
       <c r="B3" s="84" t="s">
+        <v>245</v>
+      </c>
+      <c r="C3" s="84" t="s">
         <v>246</v>
       </c>
-      <c r="C3" s="84" t="s">
+      <c r="D3" s="84" t="s">
         <v>247</v>
-      </c>
-      <c r="D3" s="84" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
@@ -19532,13 +19532,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="87" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="C4" s="88">
         <v>45609</v>
       </c>
       <c r="D4" s="70" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
@@ -20229,7 +20229,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="135" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B5" s="128">
         <v>2</v>
@@ -20249,7 +20249,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="136" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B6" s="128">
         <v>2</v>
@@ -20712,7 +20712,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="135" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B5" s="128">
         <v>1</v>
@@ -20814,7 +20814,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="135" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B10" s="128">
         <v>1</v>

</xml_diff>